<commit_message>
renamed estimate to eval regression function to make it consistent
</commit_message>
<xml_diff>
--- a/Distribution/ACQ.Options.xlsx
+++ b/Distribution/ACQ.Options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ACQ\ACQ.Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54BC0DB-928E-4FF6-A8BA-1D02D9AE1EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C52927-8748-480A-8AFF-3BB3B1A12830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="705" windowWidth="26475" windowHeight="12885" tabRatio="900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-885" yWindow="1485" windowWidth="24450" windowHeight="12690" tabRatio="900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Utils" sheetId="3" r:id="rId1"/>
@@ -13553,18 +13553,18 @@
       </c>
       <c r="C4" s="6" t="str">
         <f>_xll.acq_version()</f>
-        <v>1.3.8029.27023</v>
+        <v>1.3.8032.39391</v>
       </c>
       <c r="G4" t="s">
         <v>1</v>
       </c>
       <c r="H4" s="48">
         <f ca="1">TODAY()</f>
-        <v>44555</v>
+        <v>44558</v>
       </c>
       <c r="J4" s="49" t="str">
         <f ca="1">_xll.acq_tostring(H4)</f>
-        <v>44555</v>
+        <v>44558</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -13686,7 +13686,7 @@
       </c>
       <c r="H13" t="str">
         <f ca="1">_xll.acq_join(H3:H10)</f>
-        <v>3.14159265358979,44555,True,,,,,</v>
+        <v>3.14159265358979,44558,True,,,,,</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13695,7 +13695,7 @@
       </c>
       <c r="H14" t="str">
         <f ca="1">_xll.acq_join(J3:J10, "|")</f>
-        <v>3.14159265358979|44555|TRUE|||||</v>
+        <v>3.14159265358979|44558|TRUE|||||</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>